<commit_message>
complete upto privot data validation,sorting, filtering
</commit_message>
<xml_diff>
--- a/MS Excell/Advance.xlsx
+++ b/MS Excell/Advance.xlsx
@@ -4,16 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data Table" sheetId="1" r:id="rId1"/>
     <sheet name="Chart" sheetId="2" r:id="rId2"/>
     <sheet name="Privot Table&amp;Chart" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Validation" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chart!$C$1:$C$6</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="65" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -387,19 +391,19 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>Apple</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>bannas</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Apple</c:v>
-                  </c:pt>
                   <c:pt idx="2">
+                    <c:v>Bannas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Grapes</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Orange</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Bannas</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Grapes</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -555,19 +559,19 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>Apple</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>bannas</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Apple</c:v>
-                  </c:pt>
                   <c:pt idx="2">
+                    <c:v>Bannas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Grapes</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Orange</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Bannas</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Grapes</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -913,6 +917,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DD71-435A-AF2D-402744D16DFF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -933,6 +942,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DD71-435A-AF2D-402744D16DFF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -953,6 +967,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DD71-435A-AF2D-402744D16DFF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -973,6 +992,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-DD71-435A-AF2D-402744D16DFF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -993,6 +1017,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-DD71-435A-AF2D-402744D16DFF}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1076,19 +1105,19 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>Apple</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>bannas</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Apple</c:v>
-                  </c:pt>
                   <c:pt idx="2">
+                    <c:v>Bannas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Grapes</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Orange</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Bannas</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Grapes</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1193,6 +1222,11 @@
                       </a:contourClr>
                     </a:sp3d>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000000B-DD71-435A-AF2D-402744D16DFF}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="1"/>
@@ -1213,6 +1247,11 @@
                       </a:contourClr>
                     </a:sp3d>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000000D-DD71-435A-AF2D-402744D16DFF}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="2"/>
@@ -1233,6 +1272,11 @@
                       </a:contourClr>
                     </a:sp3d>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000000F-DD71-435A-AF2D-402744D16DFF}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="3"/>
@@ -1253,6 +1297,11 @@
                       </a:contourClr>
                     </a:sp3d>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000011-DD71-435A-AF2D-402744D16DFF}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="4"/>
@@ -1273,6 +1322,11 @@
                       </a:contourClr>
                     </a:sp3d>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000013-DD71-435A-AF2D-402744D16DFF}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dLbls>
                   <c:spPr>
@@ -1360,19 +1414,19 @@
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
+                          <c:v>Apple</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
                           <c:v>bannas</c:v>
                         </c:pt>
-                        <c:pt idx="1">
-                          <c:v>Apple</c:v>
-                        </c:pt>
                         <c:pt idx="2">
-                          <c:v>Orange</c:v>
+                          <c:v>Bannas</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>Bannas</c:v>
+                          <c:v>Grapes</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>Grapes</c:v>
+                          <c:v>Orange</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1700,19 +1754,19 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>Apple</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>bannas</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Apple</c:v>
-                  </c:pt>
                   <c:pt idx="2">
+                    <c:v>Bannas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Grapes</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Orange</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Bannas</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Grapes</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1868,19 +1922,19 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>Apple</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>bannas</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Apple</c:v>
-                  </c:pt>
                   <c:pt idx="2">
+                    <c:v>Bannas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Grapes</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Orange</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Bannas</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Grapes</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2118,7 +2172,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Data Tables.xlsx]Privot Table&amp;Chart!PivotTable50</c:name>
+    <c:name>[Advance.xlsx]Privot Table&amp;Chart!PivotTable50</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -5080,7 +5134,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="43887.955962384258" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="5">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E6" sheet="Privot Table&amp;Chart"/>
+    <worksheetSource ref="A1:E6" sheet="Privot Table&amp;Chart" r:id="rId2"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Name" numFmtId="0">
@@ -5165,7 +5219,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable50" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable50" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="E12:K18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -5321,7 +5375,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable41" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable41" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H3:N9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -5739,14 +5793,14 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <f t="dataTable" ref="C7:C12" dt2D="0" dtr="0" r1="B2"/>
+        <f t="dataTable" ref="C7:C12" dt2D="0" dtr="0" r1="B2" ca="1"/>
         <v>320</v>
       </c>
       <c r="E7">
         <v>16</v>
       </c>
       <c r="F7" s="2">
-        <f t="dataTable" ref="F7:I12" dt2D="1" dtr="1" r1="B1" r2="B2" ca="1"/>
+        <f t="dataTable" ref="F7:I12" dt2D="1" dtr="1" r1="B1" r2="B2"/>
         <v>336</v>
       </c>
       <c r="G7" s="2">
@@ -5885,7 +5939,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5912,7 +5966,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
@@ -5929,7 +5983,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>19</v>
@@ -5946,7 +6000,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>20</v>
@@ -5963,7 +6017,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
@@ -5980,7 +6034,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
@@ -5993,6 +6047,10 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C6"/>
+  <sortState ref="B2:B6">
+    <sortCondition ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6003,7 +6061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -6365,4 +6423,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Caution" error="please enter value greater than 1" promptTitle="Message" prompt="Enter value greter than 1" sqref="A1:A6">
+      <formula1>1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete upto privot data validation,sorting, filtering,vlookup,macros
</commit_message>
<xml_diff>
--- a/MS Excell/Advance.xlsx
+++ b/MS Excell/Advance.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data Table" sheetId="1" r:id="rId1"/>
     <sheet name="Chart" sheetId="2" r:id="rId2"/>
     <sheet name="Privot Table&amp;Chart" sheetId="3" r:id="rId3"/>
-    <sheet name="Data Validation" sheetId="4" r:id="rId4"/>
+    <sheet name="Cross referencing" sheetId="5" r:id="rId4"/>
+    <sheet name="reference" sheetId="6" r:id="rId5"/>
+    <sheet name="Data Validation" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chart!$C$1:$C$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
   <si>
     <t>price per glass</t>
   </si>
@@ -113,16 +115,27 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>total cost</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,10 +161,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -166,8 +180,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -251,7 +267,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -349,7 +364,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -517,7 +531,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -728,7 +741,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -810,7 +822,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1076,9 +1087,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1499,7 +1508,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1614,7 +1622,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1712,7 +1719,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1880,7 +1886,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2091,7 +2096,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2700,7 +2704,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5793,14 +5796,14 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <f t="dataTable" ref="C7:C12" dt2D="0" dtr="0" r1="B2" ca="1"/>
+        <f t="dataTable" ref="C7:C12" dt2D="0" dtr="0" r1="B2"/>
         <v>320</v>
       </c>
       <c r="E7">
         <v>16</v>
       </c>
       <c r="F7" s="2">
-        <f t="dataTable" ref="F7:I12" dt2D="1" dtr="1" r1="B1" r2="B2"/>
+        <f t="dataTable" ref="F7:I12" dt2D="1" dtr="1" r1="B1" r2="B2" ca="1"/>
         <v>336</v>
       </c>
       <c r="G7" s="2">
@@ -6062,7 +6065,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6427,9 +6430,293 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4">
+        <v>50</v>
+      </c>
+      <c r="F2" s="8">
+        <f>VLOOKUP("shahid",reference!A1:F6,6,)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>70</v>
+      </c>
+      <c r="F3" s="8">
+        <f>VLOOKUP(A3,reference!A1:F6,6,)</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" s="8">
+        <f>VLOOKUP(A4,reference!A2:F7,6,)</f>
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44</v>
+      </c>
+      <c r="E5" s="4">
+        <v>150</v>
+      </c>
+      <c r="F5" s="8">
+        <f>VLOOKUP(A5,reference!A3:F8,6,)</f>
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4">
+        <v>300</v>
+      </c>
+      <c r="F6" s="8">
+        <f>VLOOKUP(A6,reference!A4:F9,6,)</f>
+        <v>8400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*E2</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>70</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F6" si="0">D3*E3</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44</v>
+      </c>
+      <c r="E5" s="4">
+        <v>150</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4">
+        <v>300</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>8400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>